<commit_message>
Mise à jour PO
</commit_message>
<xml_diff>
--- a/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
+++ b/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Points</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Minutes</t>
   </si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>Responsable</t>
+  </si>
+  <si>
+    <t>Efforts</t>
+  </si>
+  <si>
+    <t>Priorité</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -160,6 +163,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,35 +463,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="43.9" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="58.86328125" customWidth="1"/>
-    <col min="3" max="3" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="43.9" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="43.9" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -492,10 +503,14 @@
       <c r="D3" s="2">
         <v>30</v>
       </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" ht="43.9" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -503,10 +518,14 @@
       <c r="D4" s="2">
         <v>40</v>
       </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:6" ht="43.9" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -514,10 +533,14 @@
       <c r="D5" s="2">
         <v>80</v>
       </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:6" ht="43.9" customHeight="1">
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -525,10 +548,14 @@
       <c r="D6" s="2">
         <v>120</v>
       </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" ht="43.9" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>8</v>
@@ -536,10 +563,14 @@
       <c r="D7" s="2">
         <v>100</v>
       </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" ht="43.9" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>8</v>
@@ -547,10 +578,14 @@
       <c r="D8" s="2">
         <v>100</v>
       </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" ht="43.9" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
@@ -558,10 +593,14 @@
       <c r="D9" s="2">
         <v>80</v>
       </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" ht="43.9" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -569,10 +608,14 @@
       <c r="D10" s="2">
         <v>30</v>
       </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" ht="43.9" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -580,10 +623,14 @@
       <c r="D11" s="2">
         <v>40</v>
       </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" ht="43.9" customHeight="1">
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -591,10 +638,14 @@
       <c r="D12" s="2">
         <v>80</v>
       </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" ht="43.9" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -602,10 +653,14 @@
       <c r="D13" s="2">
         <v>20</v>
       </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" ht="43.9" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -613,10 +668,14 @@
       <c r="D14" s="2">
         <v>20</v>
       </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" ht="43.9" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -624,10 +683,14 @@
       <c r="D15" s="2">
         <v>20</v>
       </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" ht="43.9" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -635,10 +698,14 @@
       <c r="D16" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" ht="43.9" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -646,10 +713,14 @@
       <c r="D17" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" ht="43.9" customHeight="1">
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -657,10 +728,14 @@
       <c r="D18" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" ht="43.9" customHeight="1">
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
         <v>2</v>
@@ -668,10 +743,14 @@
       <c r="D19" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" ht="43.9" customHeight="1">
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2">
         <v>4</v>
@@ -679,10 +758,14 @@
       <c r="D20" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" ht="43.9" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
         <v>4</v>
@@ -690,10 +773,14 @@
       <c r="D21" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="43.9" customHeight="1">
+      <c r="E21" s="5">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" ht="43.9" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <f>SUM(C3:C21)</f>
@@ -704,9 +791,9 @@
         <v>990</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="43.9" customHeight="1">
+    <row r="23" spans="2:6" ht="43.9" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23">
         <f>D22/60</f>

</xml_diff>

<commit_message>
scrum d'equipe, resultas de scrum poker
</commit_message>
<xml_diff>
--- a/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
+++ b/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\OneDrive\Desktop\Learning_to_Code\projet-developpement-applications\projet-developpement-applications\Scrum 1\Product Owner Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0595A93B-A8EF-4793-95A9-CACEF24FF787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="68" windowWidth="16470" windowHeight="13043"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -99,8 +118,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,11 +192,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +278,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +330,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,23 +523,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="43.9" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="43.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="58.86328125" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="15.1328125" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="43.9" customHeight="1">
+    <row r="2" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,224 +556,239 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="43.9" customHeight="1">
+    <row r="3" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>30</v>
+        <f>C3*60</f>
+        <v>60</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="2:6" ht="43.9" customHeight="1">
+    <row r="4" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>3</v>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>40</v>
+        <f t="shared" ref="D4:D21" si="0">C4*60</f>
+        <v>60</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="2:6" ht="43.9" customHeight="1">
+    <row r="5" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
+      <c r="C5">
+        <v>0.5</v>
       </c>
       <c r="D5" s="2">
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="2:6" ht="43.9" customHeight="1">
+    <row r="6" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
-        <v>8</v>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6" ht="43.9" customHeight="1">
+    <row r="7" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
-        <v>8</v>
+      <c r="C7">
+        <v>0.5</v>
       </c>
       <c r="D7" s="2">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="2:6" ht="43.9" customHeight="1">
+    <row r="8" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
-        <v>8</v>
+      <c r="C8">
+        <v>0.5</v>
       </c>
       <c r="D8" s="2">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="2:6" ht="43.9" customHeight="1">
+    <row r="9" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
+      <c r="C9">
+        <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="2:6" ht="43.9" customHeight="1">
+    <row r="10" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="2">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="2:6" ht="43.9" customHeight="1">
+    <row r="11" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
-        <v>3</v>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="2:6" ht="43.9" customHeight="1">
+    <row r="12" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
+      <c r="C12">
+        <v>2</v>
       </c>
       <c r="D12" s="2">
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="2:6" ht="43.9" customHeight="1">
+    <row r="13" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2">
-        <v>1</v>
+      <c r="C13">
+        <v>0.5</v>
       </c>
       <c r="D13" s="2">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="2:6" ht="43.9" customHeight="1">
+    <row r="14" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
+      <c r="C14">
+        <v>0.5</v>
       </c>
       <c r="D14" s="2">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" ht="43.9" customHeight="1">
+    <row r="15" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
+      <c r="C15">
+        <v>0.5</v>
       </c>
       <c r="D15" s="2">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:6" ht="43.9" customHeight="1">
+    <row r="16" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
+      <c r="C16">
+        <v>0.5</v>
       </c>
       <c r="D16" s="2">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:6" ht="43.9" customHeight="1">
+    <row r="17" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2">
-        <v>2</v>
+      <c r="C17">
+        <v>0.5</v>
       </c>
       <c r="D17" s="2">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E17" s="5">
@@ -718,14 +796,15 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" ht="43.9" customHeight="1">
+    <row r="18" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
-        <v>2</v>
+      <c r="C18">
+        <v>0.5</v>
       </c>
       <c r="D18" s="2">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E18" s="5">
@@ -733,71 +812,74 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="2:6" ht="43.9" customHeight="1">
+    <row r="19" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2">
-        <v>2</v>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="2:6" ht="43.9" customHeight="1">
+    <row r="20" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2">
-        <v>4</v>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20" s="2">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" ht="43.9" customHeight="1">
+    <row r="21" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="2">
-        <v>4</v>
+      <c r="C21">
+        <v>3</v>
       </c>
       <c r="D21" s="2">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
       <c r="E21" s="5">
         <v>2</v>
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="2:6" ht="43.9" customHeight="1">
+    <row r="22" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C22">
         <f>SUM(C3:C21)</f>
-        <v>67</v>
+        <v>20.5</v>
       </c>
       <c r="D22">
         <f>SUM(D3:D21)</f>
-        <v>990</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="43.9" customHeight="1">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D23">
         <f>D22/60</f>
-        <v>16.5</v>
+        <v>20.5</v>
       </c>
     </row>
   </sheetData>
@@ -806,24 +888,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
importation de fichier JSOn via l'interface avec le file explorer, lecture du fichier JSON en JArray, analyze de la regle 1. TODO: regles 2 a 7
</commit_message>
<xml_diff>
--- a/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
+++ b/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\OneDrive\Desktop\Learning_to_Code\projet-developpement-applications\projet-developpement-applications\Scrum 1\Product Owner Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0595A93B-A8EF-4793-95A9-CACEF24FF787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F52920D-04AC-4695-86CA-475800BDF891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5532" yWindow="1872" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Minutes</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Priorité</t>
+  </si>
+  <si>
+    <t>validation de numero d'emplyee dans le login </t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -186,6 +189,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="43.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -580,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D21" si="0">C4*60</f>
+        <f t="shared" ref="D4:D22" si="0">C4*60</f>
         <v>60</v>
       </c>
       <c r="E4" s="5">
@@ -861,29 +868,44 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>22</v>
+      <c r="B22" t="s">
+        <v>26</v>
       </c>
       <c r="C22">
-        <f>SUM(C3:C21)</f>
-        <v>20.5</v>
-      </c>
-      <c r="D22">
-        <f>SUM(D3:D21)</f>
-        <v>1230</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>SUM(C3:C22)</f>
+        <v>21.5</v>
+      </c>
+      <c r="D23">
+        <f>SUM(D3:D22)</f>
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23">
-        <f>D22/60</f>
-        <v>20.5</v>
+      <c r="D24">
+        <f>D23/60</f>
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correction de numero d'employe pour les administrateurs
</commit_message>
<xml_diff>
--- a/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
+++ b/Scrum 1/Product Owner Documentation/Backlog Taches01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\OneDrive\Desktop\Learning_to_Code\projet-developpement-applications\projet-developpement-applications\Scrum 1\Product Owner Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F52920D-04AC-4695-86CA-475800BDF891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465D9A25-2104-4445-8F40-6EE98B2F15E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5532" yWindow="1872" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Minutes</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Élaborer des messages d'erreur pour chaque règle enfreinte</t>
   </si>
   <si>
-    <t>Ajouter une interface de ligne de commande pour faciliter l'utilisation</t>
-  </si>
-  <si>
     <t>Heures totales Estimées</t>
   </si>
   <si>
@@ -116,6 +113,21 @@
   </si>
   <si>
     <t>validation de numero d'emplyee dans le login </t>
+  </si>
+  <si>
+    <t>Serge</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Serge, Pat</t>
+  </si>
+  <si>
+    <t>pat</t>
+  </si>
+  <si>
+    <t>Ajouter une interface GUI pour faciliter l'utilisation</t>
   </si>
 </sst>
 </file>
@@ -533,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="43.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -551,16 +563,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -577,7 +589,9 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -593,7 +607,9 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -609,7 +625,9 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -625,7 +643,9 @@
       <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -641,7 +661,9 @@
       <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -657,7 +679,9 @@
       <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -673,7 +697,9 @@
       <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -689,7 +715,9 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -705,7 +733,9 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -737,7 +767,9 @@
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -753,7 +785,9 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -769,7 +803,9 @@
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
@@ -785,7 +821,9 @@
       <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -801,7 +839,9 @@
       <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -817,7 +857,9 @@
       <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -833,7 +875,9 @@
       <c r="E19" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
@@ -853,7 +897,7 @@
     </row>
     <row r="21" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -865,11 +909,13 @@
       <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -883,7 +929,7 @@
     </row>
     <row r="23" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <f>SUM(C3:C22)</f>
@@ -896,7 +942,7 @@
     </row>
     <row r="24" spans="2:6" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24">
         <f>D23/60</f>

</xml_diff>